<commit_message>
added new GUI Feature
</commit_message>
<xml_diff>
--- a/input_csv/02_Arbeitsspeicher/artikel.xlsx
+++ b/input_csv/02_Arbeitsspeicher/artikel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico.Brosowski\Desktop\____Apps___\JTL_Apps\Open_AI_Searcher\input_csv\02_Arbeitsspeicher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBE14BB-D42E-465F-9A08-198B8953D3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166161C5-E2C2-4AEC-9AB9-9345138718DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{49964F96-7016-408A-B9F1-82EBE7E4DC19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{49964F96-7016-408A-B9F1-82EBE7E4DC19}"/>
   </bookViews>
   <sheets>
     <sheet name="Gehäuse" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Artikelname</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t>128GB DDR5-6000 CL32 G.Skill TZ5 Neo RGB</t>
+  </si>
+  <si>
+    <t>16GB DDR4 3600MHz G.Skill Ripjaws V Series - DDR4 (2x8GB)</t>
+  </si>
+  <si>
+    <t>16GB DDR4 3600MHz G.Skill Ripjaws V Series - DDR4 (1x16GB)</t>
+  </si>
+  <si>
+    <t>32GB DDR5-6000 CL30 Kingston FURY Beast Kit 2x 16GB (AMD)</t>
+  </si>
+  <si>
+    <t>32GB DDR5-6000 CL30 Kingston FURY Beast Kit 2x 16GB (INTEL)</t>
   </si>
 </sst>
 </file>
@@ -910,15 +922,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39DE48C-9215-4964-B44D-F102CDA843EF}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" customWidth="1"/>
+    <col min="1" max="1" width="54.140625" customWidth="1"/>
     <col min="2" max="2" width="47.28515625" customWidth="1"/>
     <col min="3" max="3" width="42.42578125" customWidth="1"/>
   </cols>
@@ -974,6 +986,50 @@
         <v>4711549510689</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>106547</v>
+      </c>
+      <c r="C6">
+        <v>4713294225634</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>106538</v>
+      </c>
+      <c r="C7">
+        <v>4713294230089</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>106525</v>
+      </c>
+      <c r="C8">
+        <v>740617343229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>106524</v>
+      </c>
+      <c r="C9">
+        <v>740617342994</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new GUI feature and fuction
</commit_message>
<xml_diff>
--- a/input_csv/02_Arbeitsspeicher/artikel.xlsx
+++ b/input_csv/02_Arbeitsspeicher/artikel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico.Brosowski\Desktop\____Apps___\JTL_Apps\Open_AI_Searcher\input_csv\02_Arbeitsspeicher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459399A3-AA26-4999-9902-E13880D0DA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A683CE7A-B77D-4DFE-936E-D471E094CE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{49964F96-7016-408A-B9F1-82EBE7E4DC19}"/>
   </bookViews>
@@ -928,7 +928,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>